<commit_message>
Changes have been made to Assignment and Spread Sheet
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Database Connectivity &amp; Web Services\Assignments_Phase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1492CE6A-9D6A-4193-9FB7-B23DF2EBD985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C364F2-6DD9-493F-A11C-5A7C633660ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>GitHub Link</t>
   </si>
@@ -64,13 +64,19 @@
   </si>
   <si>
     <t>https://github.com/Vasanth30e/Assignments_Phase2/tree/master/Assignment_5</t>
+  </si>
+  <si>
+    <t>Assignment_6</t>
+  </si>
+  <si>
+    <t>https://github.com/Vasanth30e/Assignments_Phase2/tree/master/Assignment_6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,9 +130,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="12"/>
-      <color theme="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -187,7 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -210,13 +222,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -500,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,6 +592,17 @@
       </c>
       <c r="C6" s="2">
         <v>45155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2">
+        <v>45156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the Spread Sheet
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Database Connectivity &amp; Web Services\Assignments_Phase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C364F2-6DD9-493F-A11C-5A7C633660ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7E0B9E-4874-44DC-8F87-C21A1D584FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>GitHub Link</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>https://github.com/Vasanth30e/Assignments_Phase2/tree/master/Assignment_6</t>
+  </si>
+  <si>
+    <t>Assignment_7</t>
+  </si>
+  <si>
+    <t>https://github.com/Vasanth30e/Assignments_Phase2/tree/master/Assignment_7</t>
   </si>
 </sst>
 </file>
@@ -199,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -232,6 +238,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -515,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,6 +614,17 @@
         <v>45156</v>
       </c>
     </row>
+    <row r="8" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2">
+        <v>45159</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -613,6 +633,7 @@
     <hyperlink ref="B4" r:id="rId3" xr:uid="{8CAAF770-E420-4D7F-B8BE-C2F5089802B7}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{0C375A62-114A-410A-9B20-EDBAE4124CC6}"/>
     <hyperlink ref="B6" r:id="rId5" xr:uid="{E73E22DC-709D-471B-8E92-EBD6583ABCEE}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{8B27154E-A55B-41AE-BF16-FDC0CF3B4718}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes made to spread sheet
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Database Connectivity &amp; Web Services\Assignments_Phase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7E0B9E-4874-44DC-8F87-C21A1D584FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DCFE23-E1B7-4333-BD51-CD7FB75CD600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>GitHub Link</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>https://github.com/Vasanth30e/Assignments_Phase2/tree/master/Assignment_7</t>
+  </si>
+  <si>
+    <t>Assignment_8</t>
+  </si>
+  <si>
+    <t>https://github.com/Vasanth30e/Assignments_Phase2/tree/master/Assignment_8</t>
   </si>
 </sst>
 </file>
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,6 +631,17 @@
         <v>45159</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2">
+        <v>45160</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -634,6 +651,7 @@
     <hyperlink ref="B5" r:id="rId4" xr:uid="{0C375A62-114A-410A-9B20-EDBAE4124CC6}"/>
     <hyperlink ref="B6" r:id="rId5" xr:uid="{E73E22DC-709D-471B-8E92-EBD6583ABCEE}"/>
     <hyperlink ref="B8" r:id="rId6" xr:uid="{8B27154E-A55B-41AE-BF16-FDC0CF3B4718}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{C69EE4AD-4234-45F0-85CC-ADC103CC7756}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CRUD in MVC Core
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Database Connectivity &amp; Web Services\Assignments_Phase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5521AF5F-3F58-4ACD-BAEE-F94E214021BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F45D0B-3CAF-4249-8A95-5465798323EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7755" yWindow="540" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7980" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>GitHub Link</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>https://github.com/Vasanth30e/Assignments_Phase2/tree/master/Assignment_14/ADO.NET_CRUD</t>
+  </si>
+  <si>
+    <t>Assignment_15</t>
+  </si>
+  <si>
+    <t>https://github.com/Vasanth30e/Assignments_Phase2/tree/master/Assignment_15/CustomErrorHandling</t>
   </si>
 </sst>
 </file>
@@ -579,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,6 +761,17 @@
       </c>
       <c r="C15" s="2">
         <v>45168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2">
+        <v>45169</v>
       </c>
     </row>
   </sheetData>
@@ -773,8 +790,9 @@
     <hyperlink ref="B13" r:id="rId11" xr:uid="{C41A4824-2CDB-4FFD-AF5A-D5A76306A060}"/>
     <hyperlink ref="B15" r:id="rId12" xr:uid="{9344C5C9-2112-4DCC-8E24-0FAFDDF9D313}"/>
     <hyperlink ref="B14" r:id="rId13" xr:uid="{0FA3E435-5827-4B6E-97A4-66D766878F01}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{05BD94D8-96EA-4515-85B1-DA56BCB9C680}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes have been commited to spread sheet
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Database Connectivity &amp; Web Services\Assignments_Phase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF5B2AA-4E95-4B19-BF07-C0E8FFAB62D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB17DA6-90EE-4FEC-9FD0-F55ED1549DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6540" yWindow="3870" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>GitHub Link</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>https://github.com/Vasanth30e/Assignments_Phase2/tree/master/Assignment_16/TaskCRUD</t>
+  </si>
+  <si>
+    <t>Assignment_17</t>
+  </si>
+  <si>
+    <t>https://github.com/Vasanth30e/Assignments_Phase2/tree/master/Assignment_17/MovieAPI</t>
   </si>
 </sst>
 </file>
@@ -591,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C18" sqref="B18:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,6 +795,17 @@
       </c>
       <c r="C17" s="2">
         <v>45170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2">
+        <v>45173</v>
       </c>
     </row>
   </sheetData>
@@ -809,8 +826,9 @@
     <hyperlink ref="B14" r:id="rId13" xr:uid="{0FA3E435-5827-4B6E-97A4-66D766878F01}"/>
     <hyperlink ref="B16" r:id="rId14" xr:uid="{05BD94D8-96EA-4515-85B1-DA56BCB9C680}"/>
     <hyperlink ref="B17" r:id="rId15" xr:uid="{1917D2CD-9B45-4205-8906-2EA0675A39CE}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{4147D39C-A12E-4A43-A5E6-6C9D94DF8799}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>